<commit_message>
ajout du PDM v1.0 + mise à jour des documents de gestion
</commit_message>
<xml_diff>
--- a/Gestion de projet/Gestion du budget.xlsx
+++ b/Gestion de projet/Gestion du budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Google Drive\M2GIL\SPORTIFS\Gestion de projet\MOE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Documents\SPORTIFS\sportifs.documents\Gestion de projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
@@ -1569,11 +1569,11 @@
       </c>
       <c r="K24" s="2">
         <f>SUM(C24:I24)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L24" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>13</v>
@@ -1590,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -1609,11 +1609,11 @@
       </c>
       <c r="K25" s="2">
         <f>SUM(C25:I25)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L25" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Mise à jour des documents (risques, traçabilité, livrables,décisions)
</commit_message>
<xml_diff>
--- a/Gestion de projet/Gestion du budget.xlsx
+++ b/Gestion de projet/Gestion du budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Google Drive\M2GIL\SPORTIFS\Gestion de projet\MOE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Google Drive\M2GIL\SPORTIFS\MOE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -243,7 +243,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +274,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -362,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -370,11 +376,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
@@ -428,6 +462,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -801,11 +841,11 @@
       </c>
       <c r="K3" s="2">
         <f t="shared" ref="K3:K8" si="0">SUM(C3:I3)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L3" s="2">
         <f>K3*250</f>
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>13</v>
@@ -828,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -841,11 +881,11 @@
       </c>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" ref="L4:L41" si="1">K4*250</f>
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
@@ -868,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -881,11 +921,11 @@
       </c>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>13</v>
@@ -908,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -921,11 +961,11 @@
       </c>
       <c r="K6" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" si="1"/>
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>13</v>
@@ -988,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1001,11 +1041,11 @@
       </c>
       <c r="K8" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>13</v>
@@ -1030,7 +1070,7 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="2"/>
@@ -1153,7 +1193,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="3">
         <v>0</v>
@@ -1166,11 +1206,11 @@
       </c>
       <c r="K13" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" si="1"/>
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>13</v>
@@ -1193,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
@@ -1206,11 +1246,11 @@
       </c>
       <c r="K14" s="2">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>13</v>
@@ -1233,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
@@ -1246,11 +1286,11 @@
       </c>
       <c r="K15" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>13</v>
@@ -1273,7 +1313,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
@@ -1286,11 +1326,11 @@
       </c>
       <c r="K16" s="2">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>13</v>
@@ -1313,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -1326,11 +1366,11 @@
       </c>
       <c r="K17" s="2">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>13</v>
@@ -1355,7 +1395,7 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" ref="F18" si="6">SUM(F12:F17)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" ref="G18" si="7">SUM(G12:G17)</f>
@@ -1476,7 +1516,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>
@@ -1489,11 +1529,11 @@
       </c>
       <c r="K22" s="2">
         <f>SUM(C22:I22)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L22" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>13</v>
@@ -1516,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="3">
         <v>0</v>
@@ -1529,11 +1569,11 @@
       </c>
       <c r="K23" s="2">
         <f>SUM(C23:I23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>13</v>
@@ -1556,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" s="3">
         <v>0</v>
@@ -1569,11 +1609,11 @@
       </c>
       <c r="K24" s="2">
         <f>SUM(C24:I24)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L24" s="2">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>13</v>
@@ -1596,7 +1636,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G25" s="3">
         <v>0</v>
@@ -1609,11 +1649,11 @@
       </c>
       <c r="K25" s="2">
         <f>SUM(C25:I25)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L25" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>13</v>
@@ -1638,7 +1678,7 @@
       </c>
       <c r="F26" s="3">
         <f t="shared" ref="F26" si="12">SUM(F20:F25)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" ref="G26" si="13">SUM(G20:G25)</f>
@@ -1670,7 +1710,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>47</v>
       </c>
@@ -1704,7 +1744,7 @@
       </c>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>48</v>
       </c>
@@ -1720,8 +1760,8 @@
       <c r="E29" s="3">
         <v>2</v>
       </c>
-      <c r="F29" s="3">
-        <v>0</v>
+      <c r="F29" s="27">
+        <v>3</v>
       </c>
       <c r="G29" s="3">
         <v>0</v>
@@ -1734,17 +1774,17 @@
       </c>
       <c r="K29" s="2">
         <f>SUM(C29:I29)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L29" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1250</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>50</v>
       </c>
@@ -1760,7 +1800,7 @@
       <c r="E30" s="3">
         <v>0</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="28">
         <v>0</v>
       </c>
       <c r="G30" s="3">
@@ -1784,7 +1824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>52</v>
       </c>
@@ -1800,8 +1840,8 @@
       <c r="E31" s="3">
         <v>2</v>
       </c>
-      <c r="F31" s="3">
-        <v>0</v>
+      <c r="F31" s="28">
+        <v>1</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
@@ -1814,17 +1854,17 @@
       </c>
       <c r="K31" s="2">
         <f>SUM(C31:I31)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L31" s="2">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>1250</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>54</v>
       </c>
@@ -1840,8 +1880,8 @@
       <c r="E32" s="3">
         <v>2</v>
       </c>
-      <c r="F32" s="3">
-        <v>0</v>
+      <c r="F32" s="28">
+        <v>2</v>
       </c>
       <c r="G32" s="3">
         <v>0</v>
@@ -1854,17 +1894,17 @@
       </c>
       <c r="K32" s="2">
         <f>SUM(C32:I32)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L32" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M32" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>56</v>
       </c>
@@ -1880,8 +1920,8 @@
       <c r="E33" s="3">
         <v>2</v>
       </c>
-      <c r="F33" s="3">
-        <v>0</v>
+      <c r="F33" s="28">
+        <v>2</v>
       </c>
       <c r="G33" s="3">
         <v>0</v>
@@ -1894,11 +1934,11 @@
       </c>
       <c r="K33" s="2">
         <f>SUM(C33:I33)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L33" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M33" s="3" t="s">
         <v>13</v>
@@ -1923,7 +1963,7 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" ref="F34" si="18">SUM(F28:F33)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" ref="G34" si="19">SUM(G28:G33)</f>
@@ -2004,7 +2044,7 @@
         <v>2</v>
       </c>
       <c r="F37" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="3">
         <v>0</v>
@@ -2017,11 +2057,11 @@
       </c>
       <c r="K37" s="2">
         <f>SUM(C37:I37)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L37" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="M37" s="3" t="s">
         <v>13</v>
@@ -2044,7 +2084,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="3">
         <v>0</v>
@@ -2057,11 +2097,11 @@
       </c>
       <c r="K38" s="2">
         <f>SUM(C38:I38)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L38" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="M38" s="3" t="s">
         <v>13</v>
@@ -2084,7 +2124,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G39" s="3">
         <v>0</v>
@@ -2097,11 +2137,11 @@
       </c>
       <c r="K39" s="2">
         <f>SUM(C39:I39)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L39" s="2">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>13</v>
@@ -2124,7 +2164,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G40" s="3">
         <v>0</v>
@@ -2137,11 +2177,11 @@
       </c>
       <c r="K40" s="2">
         <f>SUM(C40:I40)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L40" s="2">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>2250</v>
       </c>
       <c r="M40" s="3" t="s">
         <v>13</v>
@@ -2164,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="F41" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G41" s="3">
         <v>0</v>
@@ -2177,11 +2217,11 @@
       </c>
       <c r="K41" s="2">
         <f>SUM(C41:I41)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L41" s="2">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>2250</v>
       </c>
       <c r="M41" s="3" t="s">
         <v>13</v>
@@ -2206,7 +2246,7 @@
       </c>
       <c r="F42" s="3">
         <f t="shared" ref="F42" si="24">SUM(F36:F41)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G42" s="3">
         <f t="shared" ref="G42" si="25">SUM(G36:G41)</f>
@@ -2236,7 +2276,7 @@
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E46" s="19">
         <f>SUM(L3:L8)+SUM(L12:L17)+SUM(L21:L25)+SUM(L29:L33)+SUM(L37:L41)</f>
-        <v>20000</v>
+        <v>30500</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>

</xml_diff>